<commit_message>
several debug and enhancement changes
added the informed consent forms, changed has_component bug, added he
Costoc question 'allergic to food'
</commit_message>
<xml_diff>
--- a/src/SPARQL query/VICO_different_questions_Walgreens_Costco_result.xlsx
+++ b/src/SPARQL query/VICO_different_questions_Walgreens_Costco_result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuln\Documents\VICO_project\VICO\src\SPARQL query\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repo\VICO\src\SPARQL query\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated merged file, version number, and queries
</commit_message>
<xml_diff>
--- a/src/SPARQL query/VICO_different_questions_Walgreens_Costco_result.xlsx
+++ b/src/SPARQL query/VICO_different_questions_Walgreens_Costco_result.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="different" localSheetId="0">Sheet1!$A$1:$B$15</definedName>
+    <definedName name="diffrent" localSheetId="0">Sheet1!$A$1:$B$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,8 +28,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="different" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\yuln\Documents\VICO_project\VICO\src\SPARQL query\different.txt">
+  <connection id="1" name="diffrent" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\GitHub repo\VICO\src\SPARQL query\diffrent.txt">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>question whether currently sick</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>organization</t>
+  </si>
+  <si>
+    <t>question whether allergic to food</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="different" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="diffrent" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,19 +427,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -446,7 +449,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -454,7 +457,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -462,7 +465,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -470,7 +473,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -478,7 +481,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -486,15 +489,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -502,7 +505,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -510,7 +513,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -518,7 +521,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -534,7 +537,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -542,7 +545,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -550,9 +553,17 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>